<commit_message>
updated modifications spread sheet
</commit_message>
<xml_diff>
--- a/simpleXWiki Modifications.xlsx
+++ b/simpleXWiki Modifications.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marc\Dropbox\iSafetyCase\code\simpleXWiki\simpleXWiki-5.3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marc\Dropbox\iSafetyCase\code\simpleXWiki\simpleXWiki-1.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="178">
   <si>
     <t>Technique used</t>
   </si>
@@ -401,9 +401,6 @@
     <t>Display adjacent logo text</t>
   </si>
   <si>
-    <t>Used to display the facility name</t>
-  </si>
-  <si>
     <t xml:space="preserve">Allows a custom title to be displayed next to the wiki logo. </t>
   </si>
   <si>
@@ -446,9 +443,6 @@
     <t>Override title</t>
   </si>
   <si>
-    <t>So far only use is on login page, as the page is not explicity stored, and thus, does not have a title.</t>
-  </si>
-  <si>
     <t>Overrides the header $title display. Define $title within this code block to override the standard definition.</t>
   </si>
   <si>
@@ -497,9 +491,6 @@
     <t>Option to hide the left menu set using the $hideTopNavMenus variable.</t>
   </si>
   <si>
-    <t>Used for hiding menus from lower level privilege users.</t>
-  </si>
-  <si>
     <t>If $hideTopNavMenus is true, then flow around the left menu display block. Otherwise, do nothing.</t>
   </si>
   <si>
@@ -509,9 +500,6 @@
     <t>Allows overriding of the pdftoc parameter during pdf export. Becomes useful during multipage exports, where you might want the TOC on some documents, but not on others.</t>
   </si>
   <si>
-    <t>Used in our case exporter script.</t>
-  </si>
-  <si>
     <t>If #pdfTocOverride($pdfdoc) evaluates to false and pdftoc is not 0, then display the TOC. Otherwise, don't display it.</t>
   </si>
   <si>
@@ -558,9 +546,6 @@
   </si>
   <si>
     <t>If $advancedUserLock is true, evaluate $advancedUserAllowance, and set $isAdvancedUser accordingly. If not, proceed with the default "usertype" check</t>
-  </si>
-  <si>
-    <t>Used to limit the interface for lower level users.</t>
   </si>
   <si>
     <t>Contains all of the logic and control variables for SimpleXWiki</t>
@@ -676,7 +661,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -712,7 +697,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="20% - Accent1" xfId="3" builtinId="30"/>
@@ -1023,7 +1007,7 @@
   <dimension ref="A1:G61"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1037,7 +1021,7 @@
     <col min="7" max="7" width="21.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -1045,7 +1029,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1053,7 +1037,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1061,7 +1045,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -1069,7 +1053,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>30</v>
       </c>
@@ -1077,7 +1061,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>72</v>
       </c>
@@ -1085,7 +1069,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="10" t="s">
         <v>1</v>
       </c>
@@ -1104,9 +1088,8 @@
       <c r="F7" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="G7" s="19"/>
-    </row>
-    <row r="8" spans="1:7" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="8" spans="1:6" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
         <v>16</v>
       </c>
@@ -1116,7 +1099,7 @@
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
     </row>
-    <row r="9" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>3</v>
       </c>
@@ -1131,7 +1114,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="9"/>
       <c r="B10" s="9"/>
       <c r="C10" s="2" t="s">
@@ -1144,9 +1127,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="B11" s="9"/>
       <c r="C11" s="8" t="s">
@@ -1159,7 +1142,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
         <v>14</v>
       </c>
@@ -1169,7 +1152,7 @@
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
     </row>
-    <row r="13" spans="1:7" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>80</v>
       </c>
@@ -1189,7 +1172,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>15</v>
       </c>
@@ -1209,7 +1192,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
       <c r="B15" s="16" t="s">
         <v>109</v>
@@ -1227,7 +1210,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
       <c r="B16" s="17" t="s">
         <v>112</v>
@@ -1417,34 +1400,32 @@
         <v>124</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="9"/>
       <c r="B26" s="14" t="s">
         <v>125</v>
       </c>
       <c r="C26" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D26" t="s">
         <v>127</v>
       </c>
-      <c r="D26" t="s">
-        <v>128</v>
-      </c>
       <c r="E26" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="G26" s="2" t="s">
-        <v>126</v>
-      </c>
+        <v>130</v>
+      </c>
+      <c r="G26" s="2"/>
     </row>
     <row r="27" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="9"/>
       <c r="B27" s="14" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D27" t="s">
         <v>33</v>
@@ -1453,25 +1434,25 @@
         <v>13</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="9"/>
       <c r="B28" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="C28" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="C28" s="2" t="s">
-        <v>134</v>
-      </c>
       <c r="D28" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1479,7 +1460,7 @@
         <v>78</v>
       </c>
       <c r="B29" s="14" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>79</v>
@@ -1491,7 +1472,7 @@
         <v>13</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1499,10 +1480,10 @@
         <v>21</v>
       </c>
       <c r="B30" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="C30" s="8" t="s">
         <v>140</v>
-      </c>
-      <c r="C30" s="8" t="s">
-        <v>142</v>
       </c>
       <c r="D30" t="s">
         <v>44</v>
@@ -1511,19 +1492,16 @@
         <v>30</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="G30" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="5"/>
       <c r="B31" s="16" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D31" t="s">
         <v>47</v>
@@ -1532,7 +1510,7 @@
         <v>72</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -1540,10 +1518,10 @@
         <v>36</v>
       </c>
       <c r="B32" s="14" t="s">
+        <v>145</v>
+      </c>
+      <c r="C32" s="2" t="s">
         <v>147</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>149</v>
       </c>
       <c r="D32" t="s">
         <v>43</v>
@@ -1552,7 +1530,7 @@
         <v>72</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -1560,19 +1538,19 @@
         <v>35</v>
       </c>
       <c r="B33" s="14" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D33" t="s">
         <v>51</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1580,10 +1558,10 @@
         <v>22</v>
       </c>
       <c r="B34" s="14" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D34" t="s">
         <v>46</v>
@@ -1592,16 +1570,16 @@
         <v>45</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="9"/>
       <c r="B35" s="14" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D35" t="s">
         <v>53</v>
@@ -1610,21 +1588,19 @@
         <v>52</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="G35" s="2" t="s">
-        <v>158</v>
-      </c>
+        <v>156</v>
+      </c>
+      <c r="G35" s="2"/>
     </row>
     <row r="36" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
         <v>48</v>
       </c>
       <c r="B36" s="14" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="D36" t="s">
         <v>50</v>
@@ -1633,16 +1609,14 @@
         <v>49</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="G36" s="2" t="s">
-        <v>162</v>
-      </c>
+        <v>159</v>
+      </c>
+      <c r="G36" s="2"/>
     </row>
     <row r="37" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" s="9"/>
       <c r="B37" s="14" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>81</v>
@@ -1654,7 +1628,7 @@
         <v>82</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1662,7 +1636,7 @@
         <v>23</v>
       </c>
       <c r="B38" s="14" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>87</v>
@@ -1674,7 +1648,7 @@
         <v>13</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -1682,7 +1656,7 @@
         <v>24</v>
       </c>
       <c r="B39" s="14" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>39</v>
@@ -1694,16 +1668,16 @@
         <v>9</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="9"/>
       <c r="B40" s="14" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="D40" t="s">
         <v>54</v>
@@ -1712,7 +1686,7 @@
         <v>72</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
@@ -1720,25 +1694,25 @@
         <v>37</v>
       </c>
       <c r="B41" s="14" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D41" t="s">
         <v>55</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A42" s="9"/>
       <c r="B42" s="14" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>57</v>
@@ -1750,11 +1724,9 @@
         <v>9</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="G42" s="2" t="s">
-        <v>179</v>
-      </c>
+        <v>174</v>
+      </c>
+      <c r="G42" s="2"/>
     </row>
     <row r="43" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A43" s="9"/>
@@ -1787,7 +1759,7 @@
         <v>90</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -1813,7 +1785,7 @@
         <v>92</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
menuview.vm modified to include logoutRedirect variable for controlling default login redirect page
</commit_message>
<xml_diff>
--- a/simpleXWiki Modifications.xlsx
+++ b/simpleXWiki Modifications.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marc\Dropbox\iSafetyCase\code\simpleXWiki\simpleXWiki-1.0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dropbox\iSafetyCase\Code\simplexwiki\simpleXWiki-1.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="9375"/>
+    <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="9380"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="181">
   <si>
     <t>Technique used</t>
   </si>
@@ -555,6 +555,15 @@
   </si>
   <si>
     <t>AnnotationCode.Script (jsExt obj "Annotation application")</t>
+  </si>
+  <si>
+    <t>logoutRedirect</t>
+  </si>
+  <si>
+    <t>Logout redirect</t>
+  </si>
+  <si>
+    <t>Replace the value of the xredirect paramter from $xwiki.relativeRequestURL to the value of $logoutRedirect</t>
   </si>
 </sst>
 </file>
@@ -1004,24 +1013,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G61"/>
+  <dimension ref="A1:G62"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="29" customWidth="1"/>
-    <col min="2" max="2" width="32.5703125" customWidth="1"/>
-    <col min="3" max="3" width="61.140625" customWidth="1"/>
-    <col min="4" max="4" width="29.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.5703125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="52.5703125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="21.85546875" customWidth="1"/>
+    <col min="2" max="2" width="32.54296875" customWidth="1"/>
+    <col min="3" max="3" width="61.1796875" customWidth="1"/>
+    <col min="4" max="4" width="29.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.54296875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="52.54296875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="21.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="20" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -1029,7 +1038,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1037,7 +1046,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1045,7 +1054,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -1053,7 +1062,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>30</v>
       </c>
@@ -1061,7 +1070,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>72</v>
       </c>
@@ -1069,7 +1078,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A7" s="10" t="s">
         <v>1</v>
       </c>
@@ -1089,7 +1098,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A8" s="4" t="s">
         <v>16</v>
       </c>
@@ -1099,7 +1108,7 @@
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
     </row>
-    <row r="9" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A9" s="9" t="s">
         <v>3</v>
       </c>
@@ -1114,7 +1123,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="9"/>
       <c r="B10" s="9"/>
       <c r="C10" s="2" t="s">
@@ -1127,7 +1136,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="58" x14ac:dyDescent="0.35">
       <c r="A11" s="9" t="s">
         <v>177</v>
       </c>
@@ -1142,7 +1151,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" ht="17.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A12" s="4" t="s">
         <v>14</v>
       </c>
@@ -1152,7 +1161,7 @@
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
     </row>
-    <row r="13" spans="1:6" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="29.5" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A13" s="9" t="s">
         <v>80</v>
       </c>
@@ -1172,7 +1181,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A14" s="9" t="s">
         <v>15</v>
       </c>
@@ -1192,7 +1201,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A15" s="5"/>
       <c r="B15" s="16" t="s">
         <v>109</v>
@@ -1210,7 +1219,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A16" s="5"/>
       <c r="B16" s="17" t="s">
         <v>112</v>
@@ -1228,7 +1237,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A17" s="9"/>
       <c r="B17" s="16" t="s">
         <v>110</v>
@@ -1246,7 +1255,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A18" s="9"/>
       <c r="B18" s="14" t="s">
         <v>111</v>
@@ -1264,7 +1273,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A19" s="9"/>
       <c r="B19" s="18" t="s">
         <v>112</v>
@@ -1282,7 +1291,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A20" s="9"/>
       <c r="B20" s="18" t="s">
         <v>112</v>
@@ -1300,7 +1309,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A21" s="9" t="s">
         <v>17</v>
       </c>
@@ -1320,7 +1329,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A22" s="9" t="s">
         <v>18</v>
       </c>
@@ -1340,7 +1349,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A23" s="9" t="s">
         <v>76</v>
       </c>
@@ -1360,7 +1369,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A24" s="9" t="s">
         <v>19</v>
       </c>
@@ -1380,7 +1389,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A25" s="9" t="s">
         <v>20</v>
       </c>
@@ -1400,7 +1409,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26" s="9"/>
       <c r="B26" s="14" t="s">
         <v>125</v>
@@ -1419,7 +1428,7 @@
       </c>
       <c r="G26" s="2"/>
     </row>
-    <row r="27" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A27" s="9"/>
       <c r="B27" s="14" t="s">
         <v>131</v>
@@ -1437,7 +1446,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A28" s="9"/>
       <c r="B28" s="14" t="s">
         <v>132</v>
@@ -1455,7 +1464,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A29" s="9" t="s">
         <v>78</v>
       </c>
@@ -1475,7 +1484,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="9" t="s">
         <v>21</v>
       </c>
@@ -1495,7 +1504,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A31" s="5"/>
       <c r="B31" s="16" t="s">
         <v>142</v>
@@ -1513,7 +1522,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A32" s="9" t="s">
         <v>36</v>
       </c>
@@ -1533,7 +1542,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A33" s="9" t="s">
         <v>35</v>
       </c>
@@ -1553,292 +1562,310 @@
         <v>150</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A34" s="9" t="s">
         <v>22</v>
       </c>
       <c r="B34" s="14" t="s">
-        <v>151</v>
+        <v>179</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>152</v>
       </c>
       <c r="D34" t="s">
-        <v>46</v>
+        <v>178</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>45</v>
+        <v>9</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A35" s="9"/>
       <c r="B35" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="D35" t="s">
+        <v>46</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A36" s="9"/>
+      <c r="B36" s="14" t="s">
         <v>154</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="C36" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D36" t="s">
         <v>53</v>
       </c>
-      <c r="E35" s="2" t="s">
+      <c r="E36" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="F35" s="2" t="s">
+      <c r="F36" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="G35" s="2"/>
-    </row>
-    <row r="36" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A36" s="9" t="s">
+      <c r="G36" s="2"/>
+    </row>
+    <row r="37" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A37" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="B36" s="14" t="s">
+      <c r="B37" s="14" t="s">
         <v>157</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="C37" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D37" t="s">
         <v>50</v>
       </c>
-      <c r="E36" s="2" t="s">
+      <c r="E37" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="F36" s="2" t="s">
+      <c r="F37" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="G36" s="2"/>
-    </row>
-    <row r="37" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A37" s="9"/>
-      <c r="B37" s="14" t="s">
+      <c r="G37" s="2"/>
+    </row>
+    <row r="38" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A38" s="9"/>
+      <c r="B38" s="14" t="s">
         <v>160</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="C38" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D38" t="s">
         <v>83</v>
       </c>
-      <c r="E37" s="2" t="s">
+      <c r="E38" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="F37" s="2" t="s">
+      <c r="F38" s="2" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" s="9" t="s">
+    <row r="39" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A39" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B38" s="14" t="s">
+      <c r="B39" s="14" t="s">
         <v>162</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="C39" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D39" t="s">
         <v>28</v>
       </c>
-      <c r="E38" s="2" t="s">
+      <c r="E39" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F38" s="2" t="s">
+      <c r="F39" s="2" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A39" s="9" t="s">
+    <row r="40" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A40" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="B39" s="14" t="s">
+      <c r="B40" s="14" t="s">
         <v>165</v>
       </c>
-      <c r="C39" s="2" t="s">
+      <c r="C40" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D40" t="s">
         <v>38</v>
       </c>
-      <c r="E39" s="2" t="s">
+      <c r="E40" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F39" s="2" t="s">
+      <c r="F40" s="2" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A40" s="9"/>
-      <c r="B40" s="14" t="s">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A41" s="9"/>
+      <c r="B41" s="14" t="s">
         <v>167</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="C41" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D41" t="s">
         <v>54</v>
       </c>
-      <c r="E40" s="2" t="s">
+      <c r="E41" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="F40" s="2" t="s">
+      <c r="F41" s="2" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="9" t="s">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A42" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="B41" s="14" t="s">
+      <c r="B42" s="14" t="s">
         <v>169</v>
       </c>
-      <c r="C41" s="2" t="s">
+      <c r="C42" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D42" t="s">
         <v>55</v>
       </c>
-      <c r="E41" s="2" t="s">
+      <c r="E42" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="F41" s="2" t="s">
+      <c r="F42" s="2" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A42" s="9"/>
-      <c r="B42" s="14" t="s">
-        <v>173</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="D42" t="s">
-        <v>56</v>
-      </c>
-      <c r="E42" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F42" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="G42" s="2"/>
-    </row>
-    <row r="43" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A43" s="9"/>
       <c r="B43" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D43" t="s">
+        <v>56</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="G43" s="2"/>
+    </row>
+    <row r="44" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A44" s="9"/>
+      <c r="B44" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="C43" s="2" t="s">
+      <c r="C44" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="D43" t="s">
+      <c r="D44" t="s">
         <v>58</v>
       </c>
-      <c r="E43" s="2" t="s">
+      <c r="E44" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="F43" s="2" t="s">
+      <c r="F44" s="2" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A44" s="12" t="s">
+    <row r="45" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A45" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="C45" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="11" t="s">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A46" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="C45" s="2" t="s">
+      <c r="C46" s="2" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="4" t="s">
+    <row r="47" spans="1:7" ht="17.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A47" s="4" t="s">
         <v>25</v>
-      </c>
-      <c r="B46" s="15"/>
-      <c r="C46" s="6"/>
-      <c r="D46" s="7"/>
-      <c r="E46" s="6"/>
-    </row>
-    <row r="47" spans="1:7" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="4" t="s">
-        <v>42</v>
       </c>
       <c r="B47" s="15"/>
       <c r="C47" s="6"/>
       <c r="D47" s="7"/>
       <c r="E47" s="6"/>
     </row>
-    <row r="48" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="11" t="s">
+    <row r="48" spans="1:7" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A48" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B48" s="15"/>
+      <c r="C48" s="6"/>
+      <c r="D48" s="7"/>
+      <c r="E48" s="6"/>
+    </row>
+    <row r="49" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="C48" s="2" t="s">
+      <c r="C49" s="2" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="9"/>
-      <c r="B49" s="14"/>
-      <c r="C49" s="2"/>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A50" s="9"/>
       <c r="B50" s="14"/>
       <c r="C50" s="2"/>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B51" s="14"/>
       <c r="C51" s="2"/>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B52" s="14"/>
       <c r="C52" s="2"/>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B53" s="14"/>
       <c r="C53" s="2"/>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B54" s="14"/>
       <c r="C54" s="2"/>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B55" s="14"/>
       <c r="C55" s="2"/>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B56" s="14"/>
       <c r="C56" s="2"/>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B57" s="14"/>
       <c r="C57" s="2"/>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B58" s="14"/>
       <c r="C58" s="2"/>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B59" s="14"/>
       <c r="C59" s="2"/>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B60" s="14"/>
       <c r="C60" s="2"/>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B61" s="14"/>
       <c r="C61" s="2"/>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C62" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1852,7 +1879,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1864,7 +1891,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>